<commit_message>
2 Tests are now running
</commit_message>
<xml_diff>
--- a/src/test/java/com/inetbanking/testData/LoginData.xlsx
+++ b/src/test/java/com/inetbanking/testData/LoginData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25616"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25718"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9EA2F317-CD39-4778-A4C4-D4806F11FEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{057D9C0F-14B3-463D-9640-15D6ACC9455E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,22 +35,22 @@
     <t>password</t>
   </si>
   <si>
-    <t>mngr433860</t>
-  </si>
-  <si>
-    <t>hytuhas</t>
-  </si>
-  <si>
-    <t>mngr432073</t>
-  </si>
-  <si>
-    <t>ypEhysy</t>
-  </si>
-  <si>
-    <t>mngr433861</t>
-  </si>
-  <si>
-    <t>EzAjypy</t>
+    <t>mngr441516</t>
+  </si>
+  <si>
+    <t>bYmuvyp</t>
+  </si>
+  <si>
+    <t>mngr441517</t>
+  </si>
+  <si>
+    <t>nyqavyh</t>
+  </si>
+  <si>
+    <t>mngr441518</t>
+  </si>
+  <si>
+    <t>jenuben</t>
   </si>
   <si>
     <t>mngr230823</t>
@@ -69,13 +69,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -104,9 +110,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,7 +431,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -450,18 +457,18 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Data sheet updated with valid credentials only
</commit_message>
<xml_diff>
--- a/src/test/java/com/inetbanking/testData/LoginData.xlsx
+++ b/src/test/java/com/inetbanking/testData/LoginData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25718"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{057D9C0F-14B3-463D-9640-15D6ACC9455E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A961F6B4-6836-44DF-AA3B-4A6CF1EFF9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -51,18 +51,6 @@
   </si>
   <si>
     <t>jenuben</t>
-  </si>
-  <si>
-    <t>mngr230823</t>
-  </si>
-  <si>
-    <t>kasdhdh</t>
-  </si>
-  <si>
-    <t>kdfhkdhdk</t>
-  </si>
-  <si>
-    <t>kfkfkfhdkf</t>
   </si>
 </sst>
 </file>
@@ -428,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
+      <selection activeCell="A5" sqref="A5:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -472,22 +460,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>